<commit_message>
Status changed to completed excel
</commit_message>
<xml_diff>
--- a/Sprint 4/Team06Report.xlsx
+++ b/Sprint 4/Team06Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gautham P Krishnan\Desktop\cs555_assignment\cs555tm062022Fall\Sprint 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A7ACBA-7FA6-4B2B-8E31-B5AB4928E95D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DC814E-0F19-4CCE-BD3E-BB998F7BBFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19595,7 +19595,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -19683,7 +19683,7 @@
         <v>167</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>174</v>
+        <v>38</v>
       </c>
       <c r="E4">
         <v>20</v>
@@ -19712,7 +19712,7 @@
         <v>167</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>174</v>
+        <v>38</v>
       </c>
       <c r="E5">
         <v>20</v>

</xml_diff>